<commit_message>
Excel update at 10:45
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aradl\Documents\GitHub\data-to-excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dilov\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F05BFB1-B360-46A5-905E-11EB5F00D30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A4C580-6C22-4558-AC58-03AC26B4D2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{C2AB0517-8C77-45F6-8174-133D86F9B3AE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{C2AB0517-8C77-45F6-8174-133D86F9B3AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="333">
   <si>
     <t>ناوچەی لێکۆڵینەوە</t>
   </si>
@@ -904,6 +904,159 @@
   </si>
   <si>
     <t>Cinema</t>
+  </si>
+  <si>
+    <t>تاج و تەخت</t>
+  </si>
+  <si>
+    <t>Big Wash</t>
+  </si>
+  <si>
+    <t>Carwash</t>
+  </si>
+  <si>
+    <t>C.C Cafe And Rest</t>
+  </si>
+  <si>
+    <t>Kashkol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emprator Butcher </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Butcher </t>
+  </si>
+  <si>
+    <t>Baghdadi Butcher</t>
+  </si>
+  <si>
+    <t>Butcher</t>
+  </si>
+  <si>
+    <t>Qubadi Butcher</t>
+  </si>
+  <si>
+    <t>چایخانەی عومەر گەڵاڵی</t>
+  </si>
+  <si>
+    <t>چایخانە</t>
+  </si>
+  <si>
+    <t>کولێرە بە قیمەی میری سۆران</t>
+  </si>
+  <si>
+    <t>کولێرە</t>
+  </si>
+  <si>
+    <t>کەبابخانەی ئاشتی</t>
+  </si>
+  <si>
+    <t>برژاو</t>
+  </si>
+  <si>
+    <t>Hano Cars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cars Dealership </t>
+  </si>
+  <si>
+    <t>میوانی سوڵتان</t>
+  </si>
+  <si>
+    <t>کافتریا</t>
+  </si>
+  <si>
+    <t>Klil House Co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key Makers </t>
+  </si>
+  <si>
+    <t>کۆمپانیای عقاراتی ماڵی تۆ</t>
+  </si>
+  <si>
+    <t>کڕین و فرۆشتنی زەوی و موڵک</t>
+  </si>
+  <si>
+    <t>Qasr Al-Wali Hotel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titanic </t>
+  </si>
+  <si>
+    <t>Restaurant, Hotel&amp;Spa</t>
+  </si>
+  <si>
+    <t>دەرمانخانەی حفید</t>
+  </si>
+  <si>
+    <t>شیرینی تاسووق</t>
+  </si>
+  <si>
+    <t>شیرینی فرۆش</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دیزامۆ Dizamo </t>
+  </si>
+  <si>
+    <t>مارکێت</t>
+  </si>
+  <si>
+    <t>مۆبیلیاتی وایت هۆم White Home</t>
+  </si>
+  <si>
+    <t>مۆبیلیات</t>
+  </si>
+  <si>
+    <t>چەرەساتی علی بابا</t>
+  </si>
+  <si>
+    <t>چەرەس فرۆش</t>
+  </si>
+  <si>
+    <t>هەرێمی قەل</t>
+  </si>
+  <si>
+    <t>چێشتفرۆش</t>
+  </si>
+  <si>
+    <t>پاشای برنج</t>
+  </si>
+  <si>
+    <t>Tissot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tissot Watch Dealer </t>
+  </si>
+  <si>
+    <t>ماڕکێتی میلاد پێنجوێنی</t>
+  </si>
+  <si>
+    <t>ماڕکێت</t>
+  </si>
+  <si>
+    <t>هەرزان بازاری ئەژیر</t>
+  </si>
+  <si>
+    <t>هەرزان بازاڕ</t>
+  </si>
+  <si>
+    <t>شوشەواتی مەیلی</t>
+  </si>
+  <si>
+    <t>شوشەوات</t>
+  </si>
+  <si>
+    <t>ماڕکێتی گوڵی مینا</t>
+  </si>
+  <si>
+    <t>شکۆی شار</t>
+  </si>
+  <si>
+    <t>مۆبلیات</t>
   </si>
 </sst>
 </file>
@@ -914,21 +1067,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
+      <name val="Aptos Display"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -946,14 +1099,14 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
+      <name val="Aptos Display"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -1014,10 +1167,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1070,6 +1223,114 @@
         <family val="1"/>
         <scheme val="major"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
       <font>
@@ -1294,114 +1555,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2859,26 +3012,26 @@
     <dataField name="Percentage" fld="2" subtotal="count" showDataAs="percentOfTotal" baseField="2" baseItem="0" numFmtId="10"/>
   </dataFields>
   <formats count="24">
-    <format dxfId="59">
+    <format dxfId="30">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="58">
+    <format dxfId="29">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="57">
+    <format dxfId="28">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="56">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -2888,26 +3041,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="24">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="23">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="22">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -2917,26 +3070,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="18">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="17">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="16">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -2946,26 +3099,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="12">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="10">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -3159,15 +3312,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{535B594A-705A-47EE-828A-180DCD641F71}" name="Records" displayName="Records" ref="A1:I3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I3" xr:uid="{535B594A-705A-47EE-828A-180DCD641F71}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{6DDBDD14-633F-4ABA-9C76-65525EBC76D8}" uniqueName="1" name="ناو" queryTableFieldId="1" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{66AF660A-A14F-4045-B8CB-D76792F21429}" uniqueName="2" name="ناوچەی لێکۆڵینەوە" queryTableFieldId="2" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{83CC10A2-BAF8-4862-8643-B57D68F3E76E}" uniqueName="3" name="جۆری تابلۆ" queryTableFieldId="3" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{B4812699-98AF-4B65-8C00-47F579AAA5C5}" uniqueName="4" name="جۆری بازرگانی" queryTableFieldId="4" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{AF340D88-7668-4ECB-8B3B-3835501FD903}" uniqueName="5" name="شوێنی بازرگانی" queryTableFieldId="5" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{A6A791CE-3429-4B17-9898-B4D0E1551587}" uniqueName="6" name="قەبارەی تابلۆ" queryTableFieldId="6" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{C811D6B1-52D5-4059-8C0B-D302CB5D2E05}" uniqueName="7" name="شوێنی تابلۆ" queryTableFieldId="7" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{B4600758-5D6A-4315-9602-B64AD3186DFF}" uniqueName="8" name="ئاستی نرخ" queryTableFieldId="8" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{D249D5C2-3A0D-4F27-83F4-A16DBB451849}" uniqueName="9" name="Data Collector" queryTableFieldId="9" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{6DDBDD14-633F-4ABA-9C76-65525EBC76D8}" uniqueName="1" name="ناو" queryTableFieldId="1" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{66AF660A-A14F-4045-B8CB-D76792F21429}" uniqueName="2" name="ناوچەی لێکۆڵینەوە" queryTableFieldId="2" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{83CC10A2-BAF8-4862-8643-B57D68F3E76E}" uniqueName="3" name="جۆری تابلۆ" queryTableFieldId="3" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{B4812699-98AF-4B65-8C00-47F579AAA5C5}" uniqueName="4" name="جۆری بازرگانی" queryTableFieldId="4" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{AF340D88-7668-4ECB-8B3B-3835501FD903}" uniqueName="5" name="شوێنی بازرگانی" queryTableFieldId="5" dataDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{A6A791CE-3429-4B17-9898-B4D0E1551587}" uniqueName="6" name="قەبارەی تابلۆ" queryTableFieldId="6" dataDxfId="54"/>
+    <tableColumn id="7" xr3:uid="{C811D6B1-52D5-4059-8C0B-D302CB5D2E05}" uniqueName="7" name="شوێنی تابلۆ" queryTableFieldId="7" dataDxfId="53"/>
+    <tableColumn id="8" xr3:uid="{B4600758-5D6A-4315-9602-B64AD3186DFF}" uniqueName="8" name="ئاستی نرخ" queryTableFieldId="8" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{D249D5C2-3A0D-4F27-83F4-A16DBB451849}" uniqueName="9" name="Data Collector" queryTableFieldId="9" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3177,36 +3330,36 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{56CF5556-60E9-450A-96EA-2A93F7ACBA98}" name="Table1_1" displayName="Table1_1" ref="A1:I2" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I2" xr:uid="{56CF5556-60E9-450A-96EA-2A93F7ACBA98}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5457E465-1523-4F7A-8EE7-C088FE127420}" uniqueName="1" name="ناو" queryTableFieldId="1" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{ADF28F8D-AC86-4A82-B5FA-F61AC06AAE20}" uniqueName="2" name="ناوچەی لێکۆڵینەوە" queryTableFieldId="2" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{D3F2FD61-936C-462A-B719-A6516FF06D09}" uniqueName="3" name="جۆری تابلۆ" queryTableFieldId="3" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{39B60345-E43D-4C21-91CA-5E1F9E8A4771}" uniqueName="4" name="جۆری بازرگانی" queryTableFieldId="4" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{7690E405-D68D-4E56-87CF-2DF553661D0F}" uniqueName="5" name="شوێنی بازرگانی" queryTableFieldId="5" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{23EBF398-36D3-416A-AE10-6418013A5C44}" uniqueName="6" name="قەبارەی تابلۆ" queryTableFieldId="6" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{6A74790B-F5E8-411D-A20E-15B61B1218C4}" uniqueName="7" name="شوێنی تابلۆ" queryTableFieldId="7" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{76872C0E-1E31-4D1C-A141-533AE9CEA814}" uniqueName="8" name="ئاستی نرخ" queryTableFieldId="8" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{C486E8D0-D0AD-4CCB-BCC6-2A8AD3690FE4}" uniqueName="9" name="Data Collector" queryTableFieldId="9" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{5457E465-1523-4F7A-8EE7-C088FE127420}" uniqueName="1" name="ناو" queryTableFieldId="1" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{ADF28F8D-AC86-4A82-B5FA-F61AC06AAE20}" uniqueName="2" name="ناوچەی لێکۆڵینەوە" queryTableFieldId="2" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{D3F2FD61-936C-462A-B719-A6516FF06D09}" uniqueName="3" name="جۆری تابلۆ" queryTableFieldId="3" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{39B60345-E43D-4C21-91CA-5E1F9E8A4771}" uniqueName="4" name="جۆری بازرگانی" queryTableFieldId="4" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{7690E405-D68D-4E56-87CF-2DF553661D0F}" uniqueName="5" name="شوێنی بازرگانی" queryTableFieldId="5" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{23EBF398-36D3-416A-AE10-6418013A5C44}" uniqueName="6" name="قەبارەی تابلۆ" queryTableFieldId="6" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{6A74790B-F5E8-411D-A20E-15B61B1218C4}" uniqueName="7" name="شوێنی تابلۆ" queryTableFieldId="7" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{76872C0E-1E31-4D1C-A141-533AE9CEA814}" uniqueName="8" name="ئاستی نرخ" queryTableFieldId="8" dataDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{C486E8D0-D0AD-4CCB-BCC6-2A8AD3690FE4}" uniqueName="9" name="Data Collector" queryTableFieldId="9" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48AA9856-D9B9-4A1B-82A9-09E2D746EC53}" name="Table1" displayName="Table1" ref="A1:I132" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:I132" xr:uid="{48AA9856-D9B9-4A1B-82A9-09E2D746EC53}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48AA9856-D9B9-4A1B-82A9-09E2D746EC53}" name="Table1" displayName="Table1" ref="A1:I161" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A1:I161" xr:uid="{48AA9856-D9B9-4A1B-82A9-09E2D746EC53}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I132">
     <sortCondition ref="I1:I133"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{01D59742-640B-4956-AD2D-CDDEB6C2F71F}" name="ناو" dataDxfId="15"/>
-    <tableColumn id="1" xr3:uid="{0DE53E67-991B-4473-9CAA-ADC3B3F66999}" name="ناوچەی لێکۆڵینەوە" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{68B3ED75-A20F-4E5B-BB72-61BC76C692E3}" name="جۆری تابلۆ" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{AD49EE1D-B3C7-4675-992A-D5649F6F9AAB}" name="جۆری بازرگانی" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{9F32E4D9-E1A7-4924-87B7-6B6270F38B7E}" name="شوێنی بازرگانی" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{CC62B2BE-4E45-4075-8CF7-405F33A536A9}" name="قەبارەی تابلۆ" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{901BF7DC-5F97-4BDD-98E0-C457561FDA21}" name="شوێنی تابلۆ" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{13A43650-EE8B-4D11-99EE-6C0545116F5E}" name="ئاستی نرخ" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{A7F7BCA0-3E68-4671-A567-C5F908070922}" name="Data Collector" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{01D59742-640B-4956-AD2D-CDDEB6C2F71F}" name="ناو" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{0DE53E67-991B-4473-9CAA-ADC3B3F66999}" name="ناوچەی لێکۆڵینەوە" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{68B3ED75-A20F-4E5B-BB72-61BC76C692E3}" name="جۆری تابلۆ" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{AD49EE1D-B3C7-4675-992A-D5649F6F9AAB}" name="جۆری بازرگانی" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{9F32E4D9-E1A7-4924-87B7-6B6270F38B7E}" name="شوێنی بازرگانی" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{CC62B2BE-4E45-4075-8CF7-405F33A536A9}" name="قەبارەی تابلۆ" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{901BF7DC-5F97-4BDD-98E0-C457561FDA21}" name="شوێنی تابلۆ" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{13A43650-EE8B-4D11-99EE-6C0545116F5E}" name="ئاستی نرخ" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{A7F7BCA0-3E68-4671-A567-C5F908070922}" name="Data Collector" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3535,7 +3688,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3549,19 +3702,19 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -3590,7 +3743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3619,7 +3772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3664,19 +3817,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -3705,7 +3858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3744,21 +3897,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BB0C81-FE65-4E5D-9356-7842E6FE9EF2}">
-  <dimension ref="A1:M133"/>
+  <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="79" zoomScaleNormal="41" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="61" zoomScaleNormal="41" workbookViewId="0">
+      <selection activeCell="E167" sqref="E167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="23.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="22.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="35.75" style="11" customWidth="1"/>
+    <col min="1" max="9" width="35.77734375" style="11" customWidth="1"/>
     <col min="10" max="11" width="9" style="9" customWidth="1"/>
-    <col min="12" max="12" width="25.5" style="9" customWidth="1"/>
-    <col min="13" max="16384" width="8.875" style="9"/>
+    <col min="12" max="12" width="25.44140625" style="9" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
@@ -3789,7 +3942,7 @@
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>188</v>
       </c>
@@ -3818,7 +3971,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>193</v>
       </c>
@@ -3847,7 +4000,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
@@ -3875,9 +4028,9 @@
       <c r="I4" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>90</v>
       </c>
@@ -3905,9 +4058,9 @@
       <c r="I5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="K5" s="12"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>199</v>
       </c>
@@ -3936,7 +4089,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>200</v>
       </c>
@@ -3965,7 +4118,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>105</v>
       </c>
@@ -3994,7 +4147,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>87</v>
       </c>
@@ -4023,7 +4176,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>203</v>
       </c>
@@ -4052,7 +4205,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>205</v>
       </c>
@@ -4081,7 +4234,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>112</v>
       </c>
@@ -4110,7 +4263,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>110</v>
       </c>
@@ -4139,7 +4292,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>109</v>
       </c>
@@ -4168,7 +4321,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>96</v>
       </c>
@@ -4197,7 +4350,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>94</v>
       </c>
@@ -4226,7 +4379,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>92</v>
       </c>
@@ -4255,7 +4408,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>85</v>
       </c>
@@ -4284,7 +4437,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>107</v>
       </c>
@@ -4313,7 +4466,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>196</v>
       </c>
@@ -4342,7 +4495,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>202</v>
       </c>
@@ -4371,7 +4524,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>207</v>
       </c>
@@ -4400,7 +4553,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>206</v>
       </c>
@@ -4429,7 +4582,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>208</v>
       </c>
@@ -4458,7 +4611,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>187</v>
       </c>
@@ -4487,7 +4640,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>216</v>
       </c>
@@ -4516,7 +4669,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>219</v>
       </c>
@@ -4545,7 +4698,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>221</v>
       </c>
@@ -4574,7 +4727,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>223</v>
       </c>
@@ -4603,7 +4756,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>225</v>
       </c>
@@ -4632,7 +4785,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>227</v>
       </c>
@@ -4661,7 +4814,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>229</v>
       </c>
@@ -4690,7 +4843,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>231</v>
       </c>
@@ -4719,7 +4872,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>233</v>
       </c>
@@ -4748,7 +4901,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>235</v>
       </c>
@@ -4777,7 +4930,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>237</v>
       </c>
@@ -4806,7 +4959,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>239</v>
       </c>
@@ -4835,7 +4988,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>241</v>
       </c>
@@ -4864,7 +5017,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>243</v>
       </c>
@@ -4893,7 +5046,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>245</v>
       </c>
@@ -4922,7 +5075,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>246</v>
       </c>
@@ -4951,7 +5104,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>247</v>
       </c>
@@ -4980,7 +5133,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>248</v>
       </c>
@@ -5009,7 +5162,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>250</v>
       </c>
@@ -5038,7 +5191,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>252</v>
       </c>
@@ -5067,7 +5220,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>135</v>
       </c>
@@ -5096,7 +5249,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>254</v>
       </c>
@@ -5125,7 +5278,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
         <v>256</v>
       </c>
@@ -5154,7 +5307,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>258</v>
       </c>
@@ -5183,7 +5336,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
         <v>260</v>
       </c>
@@ -5212,7 +5365,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>27</v>
       </c>
@@ -5241,7 +5394,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
         <v>171</v>
       </c>
@@ -5270,7 +5423,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
         <v>45</v>
       </c>
@@ -5299,7 +5452,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
         <v>67</v>
       </c>
@@ -5328,7 +5481,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>29</v>
       </c>
@@ -5357,7 +5510,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>194</v>
       </c>
@@ -5386,7 +5539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>61</v>
       </c>
@@ -5415,7 +5568,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>69</v>
       </c>
@@ -5444,7 +5597,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>179</v>
       </c>
@@ -5473,7 +5626,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
         <v>32</v>
       </c>
@@ -5502,7 +5655,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
         <v>40</v>
       </c>
@@ -5531,7 +5684,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
         <v>169</v>
       </c>
@@ -5560,7 +5713,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
         <v>24</v>
       </c>
@@ -5589,7 +5742,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
         <v>159</v>
       </c>
@@ -5618,7 +5771,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
         <v>161</v>
       </c>
@@ -5647,7 +5800,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
         <v>165</v>
       </c>
@@ -5676,7 +5829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
         <v>59</v>
       </c>
@@ -5705,7 +5858,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
         <v>57</v>
       </c>
@@ -5734,7 +5887,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>167</v>
       </c>
@@ -5763,7 +5916,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
         <v>163</v>
       </c>
@@ -5792,7 +5945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
         <v>170</v>
       </c>
@@ -5821,7 +5974,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
         <v>75</v>
       </c>
@@ -5850,7 +6003,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
         <v>157</v>
       </c>
@@ -5879,7 +6032,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
         <v>53</v>
       </c>
@@ -5908,7 +6061,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
         <v>47</v>
       </c>
@@ -5937,7 +6090,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
         <v>63</v>
       </c>
@@ -5966,7 +6119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
         <v>73</v>
       </c>
@@ -5995,7 +6148,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
         <v>181</v>
       </c>
@@ -6024,7 +6177,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
         <v>71</v>
       </c>
@@ -6053,7 +6206,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
         <v>184</v>
       </c>
@@ -6082,7 +6235,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
         <v>51</v>
       </c>
@@ -6111,7 +6264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
         <v>173</v>
       </c>
@@ -6140,7 +6293,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
         <v>177</v>
       </c>
@@ -6169,7 +6322,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A84" s="8" t="s">
         <v>65</v>
       </c>
@@ -6198,7 +6351,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
         <v>35</v>
       </c>
@@ -6227,7 +6380,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
         <v>182</v>
       </c>
@@ -6256,7 +6409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
         <v>55</v>
       </c>
@@ -6285,7 +6438,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A88" s="8" t="s">
         <v>49</v>
       </c>
@@ -6314,7 +6467,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
         <v>185</v>
       </c>
@@ -6343,7 +6496,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
         <v>175</v>
       </c>
@@ -6372,7 +6525,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
         <v>42</v>
       </c>
@@ -6401,7 +6554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
         <v>209</v>
       </c>
@@ -6430,7 +6583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A93" s="8" t="s">
         <v>211</v>
       </c>
@@ -6459,7 +6612,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A94" s="8" t="s">
         <v>212</v>
       </c>
@@ -6488,7 +6641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A95" s="8" t="s">
         <v>214</v>
       </c>
@@ -6517,384 +6670,384 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A96" s="13" t="s">
+    <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A96" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="B96" s="13" t="s">
+      <c r="B96" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C96" s="13" t="s">
+      <c r="C96" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D96" s="13" t="s">
+      <c r="D96" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="E96" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F96" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G96" s="13" t="s">
+      <c r="E96" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F96" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G96" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="H96" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I96" s="13" t="s">
+      <c r="H96" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I96" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A97" s="13" t="s">
+    <row r="97" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A97" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="B97" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C97" s="13" t="s">
+      <c r="B97" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C97" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D97" s="13" t="s">
+      <c r="D97" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="E97" s="13" t="s">
+      <c r="E97" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F97" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G97" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H97" s="13" t="s">
+      <c r="F97" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G97" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H97" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I97" s="13" t="s">
+      <c r="I97" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A98" s="13" t="s">
+    <row r="98" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A98" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="B98" s="13" t="s">
+      <c r="B98" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C98" s="13" t="s">
+      <c r="C98" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D98" s="13" t="s">
+      <c r="D98" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="E98" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F98" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G98" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H98" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I98" s="13" t="s">
+      <c r="E98" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F98" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G98" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H98" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I98" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A99" s="13" t="s">
+    <row r="99" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A99" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="B99" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C99" s="13" t="s">
+      <c r="B99" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C99" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D99" s="13" t="s">
+      <c r="D99" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="E99" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F99" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G99" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H99" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I99" s="13" t="s">
+      <c r="E99" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F99" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H99" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I99" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A100" s="13" t="s">
+    <row r="100" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A100" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="B100" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C100" s="13" t="s">
+      <c r="B100" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C100" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D100" s="13" t="s">
+      <c r="D100" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="E100" s="13" t="s">
+      <c r="E100" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F100" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G100" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H100" s="13" t="s">
+      <c r="F100" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G100" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H100" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I100" s="13" t="s">
+      <c r="I100" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A101" s="13" t="s">
+    <row r="101" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A101" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="B101" s="13" t="s">
+      <c r="B101" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C101" s="13" t="s">
+      <c r="C101" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D101" s="13" t="s">
+      <c r="D101" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="E101" s="13" t="s">
+      <c r="E101" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F101" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G101" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H101" s="13" t="s">
+      <c r="F101" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G101" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H101" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I101" s="13" t="s">
+      <c r="I101" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A102" s="13" t="s">
+    <row r="102" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A102" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="B102" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C102" s="13" t="s">
+      <c r="B102" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C102" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D102" s="13" t="s">
+      <c r="D102" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="E102" s="13" t="s">
+      <c r="E102" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F102" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G102" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H102" s="13" t="s">
+      <c r="F102" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G102" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H102" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I102" s="13" t="s">
+      <c r="I102" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A103" s="13" t="s">
+    <row r="103" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A103" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="B103" s="13" t="s">
+      <c r="B103" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C103" s="13" t="s">
+      <c r="C103" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D103" s="13" t="s">
+      <c r="D103" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="E103" s="13" t="s">
+      <c r="E103" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F103" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G103" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H103" s="13" t="s">
+      <c r="F103" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H103" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I103" s="13" t="s">
+      <c r="I103" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A104" s="13" t="s">
+    <row r="104" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A104" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="B104" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C104" s="13" t="s">
+      <c r="B104" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C104" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D104" s="13" t="s">
+      <c r="D104" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="E104" s="13" t="s">
+      <c r="E104" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F104" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G104" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H104" s="13" t="s">
+      <c r="F104" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G104" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H104" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I104" s="13" t="s">
+      <c r="I104" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A105" s="13" t="s">
+    <row r="105" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A105" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="B105" s="13" t="s">
+      <c r="B105" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="C105" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D105" s="13" t="s">
+      <c r="D105" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="E105" s="13" t="s">
+      <c r="E105" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F105" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G105" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H105" s="13" t="s">
+      <c r="F105" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G105" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H105" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I105" s="13" t="s">
+      <c r="I105" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A106" s="13" t="s">
+    <row r="106" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A106" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="B106" s="13" t="s">
+      <c r="B106" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C106" s="13" t="s">
+      <c r="C106" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D106" s="13" t="s">
+      <c r="D106" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="E106" s="13" t="s">
+      <c r="E106" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F106" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G106" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H106" s="13" t="s">
+      <c r="F106" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G106" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H106" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I106" s="13" t="s">
+      <c r="I106" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A107" s="13" t="s">
+    <row r="107" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A107" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="B107" s="13" t="s">
+      <c r="B107" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C107" s="13" t="s">
+      <c r="C107" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D107" s="13" t="s">
+      <c r="D107" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="E107" s="13" t="s">
+      <c r="E107" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F107" s="13" t="s">
+      <c r="F107" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="G107" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H107" s="13" t="s">
+      <c r="G107" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H107" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I107" s="13" t="s">
+      <c r="I107" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A108" s="13" t="s">
+    <row r="108" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A108" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="B108" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C108" s="13" t="s">
+      <c r="B108" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C108" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D108" s="13" t="s">
+      <c r="D108" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="E108" s="13" t="s">
+      <c r="E108" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F108" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G108" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H108" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I108" s="13" t="s">
+      <c r="F108" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G108" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H108" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I108" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
         <v>198</v>
       </c>
@@ -6923,7 +7076,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A110" s="8" t="s">
         <v>197</v>
       </c>
@@ -6952,7 +7105,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A111" s="8" t="s">
         <v>189</v>
       </c>
@@ -6981,7 +7134,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A112" s="8" t="s">
         <v>133</v>
       </c>
@@ -7010,7 +7163,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A113" s="8" t="s">
         <v>192</v>
       </c>
@@ -7039,7 +7192,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A114" s="8" t="s">
         <v>131</v>
       </c>
@@ -7068,7 +7221,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A115" s="8" t="s">
         <v>191</v>
       </c>
@@ -7097,7 +7250,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A116" s="8" t="s">
         <v>138</v>
       </c>
@@ -7126,7 +7279,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A117" s="8" t="s">
         <v>204</v>
       </c>
@@ -7155,7 +7308,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A118" s="8" t="s">
         <v>195</v>
       </c>
@@ -7184,7 +7337,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A119" s="8" t="s">
         <v>123</v>
       </c>
@@ -7213,7 +7366,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A120" s="8" t="s">
         <v>126</v>
       </c>
@@ -7242,7 +7395,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A121" s="8" t="s">
         <v>201</v>
       </c>
@@ -7271,7 +7424,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A122" s="8" t="s">
         <v>151</v>
       </c>
@@ -7300,7 +7453,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A123" s="8" t="s">
         <v>141</v>
       </c>
@@ -7329,7 +7482,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A124" s="8" t="s">
         <v>150</v>
       </c>
@@ -7358,7 +7511,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A125" s="8" t="s">
         <v>144</v>
       </c>
@@ -7387,7 +7540,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A126" s="8" t="s">
         <v>148</v>
       </c>
@@ -7416,7 +7569,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A127" s="8" t="s">
         <v>146</v>
       </c>
@@ -7445,7 +7598,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A128" s="8" t="s">
         <v>186</v>
       </c>
@@ -7474,7 +7627,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
         <v>121</v>
       </c>
@@ -7503,7 +7656,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A130" s="8" t="s">
         <v>114</v>
       </c>
@@ -7532,7 +7685,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
         <v>117</v>
       </c>
@@ -7561,7 +7714,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A132" s="8" t="s">
         <v>190</v>
       </c>
@@ -7590,16 +7743,846 @@
         <v>116</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A133"/>
-      <c r="B133"/>
-      <c r="C133"/>
-      <c r="D133"/>
-      <c r="E133"/>
-      <c r="F133"/>
-      <c r="G133"/>
-      <c r="H133"/>
-      <c r="I133"/>
+    <row r="133" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A133" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C133" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D133" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E133" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F133" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G133" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H133" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I133" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A134" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B134" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D134" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="E134" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F134" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G134" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H134" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I134" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A135" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C135" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D135" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E135" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F135" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G135" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H135" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I135" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A136" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C136" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D136" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E136" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F136" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G136" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H136" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I136" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A137" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C137" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D137" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="E137" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F137" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G137" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H137" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I137" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A138" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D138" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="E138" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F138" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G138" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H138" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I138" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A139" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C139" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D139" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="E139" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F139" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G139" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H139" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I139" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A140" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D140" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="E140" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F140" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G140" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H140" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I140" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A141" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C141" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D141" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="E141" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F141" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G141" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H141" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I141" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A142" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C142" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D142" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E142" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F142" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G142" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H142" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I142" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A143" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C143" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D143" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="E143" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F143" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G143" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H143" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I143" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A144" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B144" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C144" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D144" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="E144" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F144" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G144" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H144" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I144" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A145" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C145" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D145" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="E145" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F145" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G145" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H145" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I145" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A146" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="B146" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C146" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D146" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="E146" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F146" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G146" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H146" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I146" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A147" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C147" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D147" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="E147" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F147" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G147" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H147" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I147" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A148" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="B148" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C148" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D148" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="E148" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F148" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G148" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H148" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I148" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A149" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C149" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D149" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E149" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F149" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G149" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H149" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I149" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A150" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C150" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D150" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="E150" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F150" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G150" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H150" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I150" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A151" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C151" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D151" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="E151" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F151" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G151" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H151" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I151" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A152" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C152" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D152" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="E152" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F152" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G152" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H152" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I152" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A153" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D153" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="E153" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F153" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G153" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H153" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I153" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A154" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="B154" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C154" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D154" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="E154" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F154" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G154" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H154" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I154" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A155" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C155" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D155" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E155" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F155" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G155" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H155" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I155" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A156" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="B156" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D156" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="E156" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F156" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G156" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="H156" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I156" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A157" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="B157" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D157" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="E157" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F157" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G157" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H157" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I157" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A158" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D158" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="E158" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F158" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G158" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H158" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I158" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A159" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C159" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D159" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="E159" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F159" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G159" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H159" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I159" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A160" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C160" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D160" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="E160" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F160" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G160" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H160" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I160" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A161" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C161" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D161" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="E161" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F161" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G161" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H161" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I161" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7610,19 +8593,19 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{66D142FD-4E01-4F47-9F13-33047B87C17C}">
       <formula1>"گەورە,مامناوەند,پچووک"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G45 G49:G132 G134:G1048576" xr:uid="{52FA5747-FDD6-46D5-B658-7CAF9F4B1443}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G45 G49:G132 G143:G1048576" xr:uid="{52FA5747-FDD6-46D5-B658-7CAF9F4B1443}">
       <formula1>"سەرشەقام,ناو مۆڵ,کۆڵان,ناوبازاڕ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B132 B134:B1048576" xr:uid="{F4E3B7F3-4007-4AB1-8573-589BB09E1589}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{F4E3B7F3-4007-4AB1-8573-589BB09E1589}">
       <formula1>"جادەی سەرەکی,ناوچەی بازرگانی,ناوەندی فرۆشتن"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C132 C134:C1048576" xr:uid="{CA43A216-A0C1-439F-A94A-646899314D30}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{CA43A216-A0C1-439F-A94A-646899314D30}">
       <formula1>"تابلۆی تەواو کوردی,تابلۆی تەواو بیانی,تابلۆی تێکەڵ,تابلۆی بەناو بیانی و نووسینی کوردی"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E132 E134:E1048576" xr:uid="{C76832AF-D59E-47FA-8DEF-C13DE72F57F8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{C76832AF-D59E-47FA-8DEF-C13DE72F57F8}">
       <formula1>"ناوچەی گران,ناوچەی مامناوەند,ناوچەی هەژار"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H132 H134:H1048576" xr:uid="{9AAAC0F3-9C9D-4517-ACCF-BE4D51CD0BEB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{9AAAC0F3-9C9D-4517-ACCF-BE4D51CD0BEB}">
       <formula1>"هەرزان,مامناوەند,گران"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7640,7 +8623,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7654,20 +8637,20 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -7678,7 +8661,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -7689,7 +8672,7 @@
         <v>0.40336134453781514</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
@@ -7700,7 +8683,7 @@
         <v>0.10084033613445378</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
@@ -7711,7 +8694,7 @@
         <v>0.25210084033613445</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
@@ -7722,7 +8705,7 @@
         <v>0.24369747899159663</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -7733,7 +8716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:3" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7747,14 +8730,14 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -7764,7 +8747,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -7774,7 +8757,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -7790,7 +8773,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
@@ -7806,7 +8789,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>79</v>
       </c>
@@ -7822,7 +8805,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>116</v>
       </c>
@@ -7838,7 +8821,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>125</v>
       </c>
@@ -7854,7 +8837,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>130</v>
       </c>
@@ -7870,7 +8853,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>140</v>
       </c>
@@ -7886,7 +8869,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>143</v>
       </c>
@@ -7902,7 +8885,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>156</v>
       </c>
@@ -7918,7 +8901,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>218</v>
       </c>
@@ -7934,7 +8917,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>20</v>
       </c>
@@ -7950,7 +8933,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -7960,7 +8943,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -7970,7 +8953,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -7980,7 +8963,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -7990,7 +8973,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -8000,7 +8983,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -8010,7 +8993,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -8020,7 +9003,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -8030,7 +9013,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -8040,7 +9023,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -8050,7 +9033,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -8060,7 +9043,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -8070,7 +9053,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -8080,7 +9063,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -8090,7 +9073,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -8100,7 +9083,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -8110,7 +9093,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -8120,7 +9103,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -8130,7 +9113,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -8140,7 +9123,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -8150,7 +9133,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -8160,7 +9143,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>

</xml_diff>